<commit_message>
complete the house data by coredata
</commit_message>
<xml_diff>
--- a/excels/houseConfig.xlsx
+++ b/excels/houseConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10802"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/haoyun/Documents/XcodeProjects/myDream/excels/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nancy.shi/Documents/Life/XcodeProjects/myDream/excels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A2669-077B-404F-B233-6FED69D1FF32}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305C3FEB-8C7E-3648-85FF-928A45E6073A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11440" yWindow="2440" windowWidth="31660" windowHeight="19960" activeTab="1" xr2:uid="{B77A66DE-55A1-7342-87D7-BEF7ECBC237D}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="27820" windowHeight="17540" xr2:uid="{B77A66DE-55A1-7342-87D7-BEF7ECBC237D}"/>
   </bookViews>
   <sheets>
     <sheet name="houseConfig" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -101,6 +101,10 @@
   </si>
   <si>
     <t>dollorForInteract</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sortOrder</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -465,10 +469,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE7FDF80-E2AC-1044-B06E-3C8D8BBDD011}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -479,7 +483,7 @@
     <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,8 +505,11 @@
       <c r="G1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -524,8 +531,11 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="H2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>1001</v>
       </c>
@@ -547,8 +557,11 @@
       <c r="G3">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
       <c r="A4">
         <v>1002</v>
       </c>
@@ -570,8 +583,11 @@
       <c r="G4">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="H4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5">
         <v>1003</v>
       </c>
@@ -592,6 +608,9 @@
       </c>
       <c r="G5">
         <v>2000</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -605,8 +624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BF95008-4864-C544-97A1-E26FCB7D822C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScale="139" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>

</xml_diff>